<commit_message>
Added numbers in remainder report
</commit_message>
<xml_diff>
--- a/names.xlsx
+++ b/names.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,63 +429,63 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Кнопки</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Iphone</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Страховки</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Подписки</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Услуги</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>КЭО</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Гаджеты</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Модемы</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Аксы</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
           <t>Сим_карты</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Кнопки</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Iphone</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Страховки</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Подписки</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Услуги</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>КЭО</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Гаджеты</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Модемы</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Аксы</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Сазонов</t>
+          <t>Цыгина</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14733.5</v>
+        <v>54078.95</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -521,7 +521,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Сухарев</t>
+          <t>Чернокрылюк</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -561,7 +561,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Плетникова</t>
+          <t>Лямзина</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -601,7 +601,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Куликова</t>
+          <t>Морозова</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -681,7 +681,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Романцова</t>
+          <t>Суворов</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -761,7 +761,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Боницкий</t>
+          <t>Кузякин</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -841,7 +841,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Суворов</t>
+          <t>Куликова</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -961,7 +961,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Морозова</t>
+          <t>Романцова</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -1041,7 +1041,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Илюхина</t>
+          <t>Винокуров</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1081,7 +1081,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Тяпин</t>
+          <t>Носова</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1161,7 +1161,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Кузякин</t>
+          <t>Буянова</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1201,7 +1201,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Буянова</t>
+          <t>Мелкумян</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1241,7 +1241,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Калугина</t>
+          <t>Боницкий</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1281,7 +1281,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Винокуров</t>
+          <t>Светов</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1321,7 +1321,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Мелкумян</t>
+          <t>Кусочкова</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1361,7 +1361,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Калашникова</t>
+          <t>Чекушкин</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1401,7 +1401,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Чекушкин</t>
+          <t>Рогачев</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1441,7 +1441,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Михайлова</t>
+          <t>Илюхина</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1481,7 +1481,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Цыгина</t>
+          <t>Караганская</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1521,7 +1521,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Караганская</t>
+          <t>Калашникова</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1561,7 +1561,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Хохлова</t>
+          <t>Калугина</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1601,7 +1601,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Носова</t>
+          <t>Плетникова</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1641,7 +1641,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Чернокрылюк</t>
+          <t>Хохлова</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1681,7 +1681,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Винокуров</t>
+          <t>Тяпин</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1721,7 +1721,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Лямзина</t>
+          <t>Сытин</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1761,7 +1761,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Сытин</t>
+          <t>Голованов</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1801,7 +1801,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Голованов</t>
+          <t>Кузнецов</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1841,7 +1841,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Светов</t>
+          <t>Винокуров</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1881,7 +1881,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Рогачев</t>
+          <t>Михайлова</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -1921,7 +1921,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Кузнецов</t>
+          <t>Сазонов</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1961,7 +1961,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Кусочкова</t>
+          <t>Александр</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -2001,7 +2001,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Швецова</t>
+          <t>Сухарев</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -2081,7 +2081,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Миронова</t>
+          <t>Виктория</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -2121,7 +2121,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Сорманова</t>
+          <t>Миронова</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -2161,7 +2161,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Шувалова</t>
+          <t>Белозерова</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -2201,7 +2201,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Белозерова</t>
+          <t>Сироткин</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -2275,6 +2275,206 @@
         <v>0</v>
       </c>
       <c r="L46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Сорманова</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0</v>
+      </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Шувалова</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Смирнова</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>0</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Кочетова</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Швецова</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>